<commit_message>
USAID WCS analysis for SPR
</commit_message>
<xml_diff>
--- a/data/LengthData_20230712_EScleaned.xlsx
+++ b/data/LengthData_20230712_EScleaned.xlsx
@@ -1623,7 +1623,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Tylosurus crocodilus</t>
+          <t>Tylosurus crocodilus</t>
         </is>
       </c>
       <c r="L21">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Tylosurus crocodilus</t>
+          <t>Tylosurus crocodilus</t>
         </is>
       </c>
       <c r="L22">
@@ -5763,7 +5763,7 @@
       </c>
       <c r="K90" t="inlineStr">
         <is>
-          <t>Carangoides ciliarius</t>
+          <t>Carangoides ciliarius</t>
         </is>
       </c>
       <c r="L90">
@@ -5823,7 +5823,7 @@
       </c>
       <c r="K91" t="inlineStr">
         <is>
-          <t>Carangoides ciliarius</t>
+          <t>Carangoides ciliarius</t>
         </is>
       </c>
       <c r="L91">
@@ -5883,7 +5883,7 @@
       </c>
       <c r="K92" t="inlineStr">
         <is>
-          <t>Carangoides ciliarius</t>
+          <t>Carangoides ciliarius</t>
         </is>
       </c>
       <c r="L92">
@@ -6183,7 +6183,7 @@
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L97">
@@ -6243,7 +6243,7 @@
       </c>
       <c r="K98" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L98">
@@ -6303,7 +6303,7 @@
       </c>
       <c r="K99" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L99">
@@ -6363,7 +6363,7 @@
       </c>
       <c r="K100" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L100">
@@ -6423,7 +6423,7 @@
       </c>
       <c r="K101" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L101">
@@ -6483,7 +6483,7 @@
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L102">
@@ -6543,7 +6543,7 @@
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L103">
@@ -6603,7 +6603,7 @@
       </c>
       <c r="K104" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L104">
@@ -6663,7 +6663,7 @@
       </c>
       <c r="K105" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L105">
@@ -6723,7 +6723,7 @@
       </c>
       <c r="K106" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L106">
@@ -6783,7 +6783,7 @@
       </c>
       <c r="K107" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L107">
@@ -6843,7 +6843,7 @@
       </c>
       <c r="K108" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L108">
@@ -6903,7 +6903,7 @@
       </c>
       <c r="K109" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L109">
@@ -6963,7 +6963,7 @@
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L110">
@@ -7023,7 +7023,7 @@
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L111">
@@ -7083,7 +7083,7 @@
       </c>
       <c r="K112" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L112">
@@ -7143,7 +7143,7 @@
       </c>
       <c r="K113" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L113">
@@ -7203,7 +7203,7 @@
       </c>
       <c r="K114" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L114">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="K115" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L115">
@@ -7323,7 +7323,7 @@
       </c>
       <c r="K116" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L116">
@@ -7383,7 +7383,7 @@
       </c>
       <c r="K117" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L117">
@@ -7443,7 +7443,7 @@
       </c>
       <c r="K118" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L118">
@@ -7503,7 +7503,7 @@
       </c>
       <c r="K119" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L119">
@@ -7563,7 +7563,7 @@
       </c>
       <c r="K120" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L120">
@@ -7623,7 +7623,7 @@
       </c>
       <c r="K121" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L121">
@@ -7683,7 +7683,7 @@
       </c>
       <c r="K122" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L122">
@@ -7743,7 +7743,7 @@
       </c>
       <c r="K123" t="inlineStr">
         <is>
-          <t>Carangoides malabaricus</t>
+          <t>Carangoides malabaricus</t>
         </is>
       </c>
       <c r="L123">
@@ -7803,7 +7803,7 @@
       </c>
       <c r="K124" t="inlineStr">
         <is>
-          <t>Decapterus kurroides</t>
+          <t>Decapterus kurroides</t>
         </is>
       </c>
       <c r="L124">
@@ -7863,7 +7863,7 @@
       </c>
       <c r="K125" t="inlineStr">
         <is>
-          <t>Decapterus kurroides</t>
+          <t>Decapterus kurroides</t>
         </is>
       </c>
       <c r="L125">
@@ -7923,7 +7923,7 @@
       </c>
       <c r="K126" t="inlineStr">
         <is>
-          <t>Decapterus kurroides</t>
+          <t>Decapterus kurroides</t>
         </is>
       </c>
       <c r="L126">
@@ -8163,7 +8163,7 @@
       </c>
       <c r="K130" t="inlineStr">
         <is>
-          <t>Scomberoides tol</t>
+          <t>Scomberoides tol</t>
         </is>
       </c>
       <c r="L130">
@@ -8223,7 +8223,7 @@
       </c>
       <c r="K131" t="inlineStr">
         <is>
-          <t>Scomberoides tol</t>
+          <t>Scomberoides tol</t>
         </is>
       </c>
       <c r="L131">
@@ -8283,7 +8283,7 @@
       </c>
       <c r="K132" t="inlineStr">
         <is>
-          <t>Scomberoides tol</t>
+          <t>Scomberoides tol</t>
         </is>
       </c>
       <c r="L132">
@@ -8343,7 +8343,7 @@
       </c>
       <c r="K133" t="inlineStr">
         <is>
-          <t>Scomberoides tol</t>
+          <t>Scomberoides tol</t>
         </is>
       </c>
       <c r="L133">
@@ -8403,7 +8403,7 @@
       </c>
       <c r="K134" t="inlineStr">
         <is>
-          <t>Scomberoides tol</t>
+          <t>Scomberoides tol</t>
         </is>
       </c>
       <c r="L134">
@@ -8463,7 +8463,7 @@
       </c>
       <c r="K135" t="inlineStr">
         <is>
-          <t>Scomberoides tol</t>
+          <t>Scomberoides tol</t>
         </is>
       </c>
       <c r="L135">
@@ -8523,7 +8523,7 @@
       </c>
       <c r="K136" t="inlineStr">
         <is>
-          <t>Scomberoides tol</t>
+          <t>Scomberoides tol</t>
         </is>
       </c>
       <c r="L136">
@@ -8583,7 +8583,7 @@
       </c>
       <c r="K137" t="inlineStr">
         <is>
-          <t>Scomberoides tol</t>
+          <t>Scomberoides tol</t>
         </is>
       </c>
       <c r="L137">
@@ -8643,7 +8643,7 @@
       </c>
       <c r="K138" t="inlineStr">
         <is>
-          <t>Scomberoides tol</t>
+          <t>Scomberoides tol</t>
         </is>
       </c>
       <c r="L138">
@@ -10623,7 +10623,7 @@
       </c>
       <c r="K171" t="inlineStr">
         <is>
-          <t>Platax teira</t>
+          <t>Platax teira</t>
         </is>
       </c>
       <c r="L171">
@@ -10683,7 +10683,7 @@
       </c>
       <c r="K172" t="inlineStr">
         <is>
-          <t>Platax teira</t>
+          <t>Platax teira</t>
         </is>
       </c>
       <c r="L172">
@@ -10743,7 +10743,7 @@
       </c>
       <c r="K173" t="inlineStr">
         <is>
-          <t>Platax teira</t>
+          <t>Platax teira</t>
         </is>
       </c>
       <c r="L173">
@@ -16683,7 +16683,7 @@
       </c>
       <c r="K272" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L272">
@@ -16743,7 +16743,7 @@
       </c>
       <c r="K273" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L273">
@@ -16803,7 +16803,7 @@
       </c>
       <c r="K274" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L274">
@@ -16863,7 +16863,7 @@
       </c>
       <c r="K275" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L275">
@@ -16923,7 +16923,7 @@
       </c>
       <c r="K276" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L276">
@@ -16983,7 +16983,7 @@
       </c>
       <c r="K277" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L277">
@@ -17043,7 +17043,7 @@
       </c>
       <c r="K278" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L278">
@@ -17103,7 +17103,7 @@
       </c>
       <c r="K279" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L279">
@@ -17163,7 +17163,7 @@
       </c>
       <c r="K280" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L280">
@@ -17223,7 +17223,7 @@
       </c>
       <c r="K281" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L281">
@@ -17283,7 +17283,7 @@
       </c>
       <c r="K282" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L282">
@@ -17343,7 +17343,7 @@
       </c>
       <c r="K283" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L283">
@@ -17403,7 +17403,7 @@
       </c>
       <c r="K284" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L284">
@@ -17463,7 +17463,7 @@
       </c>
       <c r="K285" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L285">
@@ -17523,7 +17523,7 @@
       </c>
       <c r="K286" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L286">
@@ -17583,7 +17583,7 @@
       </c>
       <c r="K287" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L287">
@@ -17643,7 +17643,7 @@
       </c>
       <c r="K288" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L288">
@@ -17703,7 +17703,7 @@
       </c>
       <c r="K289" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L289">
@@ -17763,7 +17763,7 @@
       </c>
       <c r="K290" t="inlineStr">
         <is>
-          <t>Hyporhamphus affinis</t>
+          <t>Hyporhamphus affinis</t>
         </is>
       </c>
       <c r="L290">
@@ -18423,7 +18423,7 @@
       </c>
       <c r="K301" t="inlineStr">
         <is>
-          <t>Cheilinus trilobatus</t>
+          <t>Cheilinus trilobatus</t>
         </is>
       </c>
       <c r="L301">
@@ -18483,7 +18483,7 @@
       </c>
       <c r="K302" t="inlineStr">
         <is>
-          <t>Cheilinus trilobatus</t>
+          <t>Cheilinus trilobatus</t>
         </is>
       </c>
       <c r="L302">
@@ -18543,7 +18543,7 @@
       </c>
       <c r="K303" t="inlineStr">
         <is>
-          <t>Cheilinus trilobatus</t>
+          <t>Cheilinus trilobatus</t>
         </is>
       </c>
       <c r="L303">
@@ -18603,7 +18603,7 @@
       </c>
       <c r="K304" t="inlineStr">
         <is>
-          <t>Cheilinus trilobatus</t>
+          <t>Cheilinus trilobatus</t>
         </is>
       </c>
       <c r="L304">
@@ -33363,7 +33363,7 @@
       </c>
       <c r="K550" t="inlineStr">
         <is>
-          <t>Monodactylus argenteus</t>
+          <t>Monodactylus argenteus</t>
         </is>
       </c>
       <c r="L550">
@@ -33423,7 +33423,7 @@
       </c>
       <c r="K551" t="inlineStr">
         <is>
-          <t>Monodactylus argenteus</t>
+          <t>Monodactylus argenteus</t>
         </is>
       </c>
       <c r="L551">
@@ -33483,7 +33483,7 @@
       </c>
       <c r="K552" t="inlineStr">
         <is>
-          <t>Mulloidichthys vanicolensis</t>
+          <t>Mulloidichthys vanicolensis</t>
         </is>
       </c>
       <c r="L552">
@@ -33543,7 +33543,7 @@
       </c>
       <c r="K553" t="inlineStr">
         <is>
-          <t>Mulloidichthys vanicolensis</t>
+          <t>Mulloidichthys vanicolensis</t>
         </is>
       </c>
       <c r="L553">
@@ -33603,7 +33603,7 @@
       </c>
       <c r="K554" t="inlineStr">
         <is>
-          <t>Mulloidichthys vanicolensis</t>
+          <t>Mulloidichthys vanicolensis</t>
         </is>
       </c>
       <c r="L554">
@@ -37863,7 +37863,7 @@
       </c>
       <c r="K625" t="inlineStr">
         <is>
-          <t>Upeneus sulphureus</t>
+          <t>Upeneus sulphureus</t>
         </is>
       </c>
       <c r="L625">
@@ -37923,7 +37923,7 @@
       </c>
       <c r="K626" t="inlineStr">
         <is>
-          <t>Upeneus vittatus</t>
+          <t>Upeneus vittatus</t>
         </is>
       </c>
       <c r="L626">
@@ -37983,7 +37983,7 @@
       </c>
       <c r="K627" t="inlineStr">
         <is>
-          <t>Upeneus vittatus</t>
+          <t>Upeneus vittatus</t>
         </is>
       </c>
       <c r="L627">
@@ -38043,7 +38043,7 @@
       </c>
       <c r="K628" t="inlineStr">
         <is>
-          <t>Upeneus vittatus</t>
+          <t>Upeneus vittatus</t>
         </is>
       </c>
       <c r="L628">
@@ -38103,7 +38103,7 @@
       </c>
       <c r="K629" t="inlineStr">
         <is>
-          <t>Upeneus vittatus</t>
+          <t>Upeneus vittatus</t>
         </is>
       </c>
       <c r="L629">
@@ -38163,7 +38163,7 @@
       </c>
       <c r="K630" t="inlineStr">
         <is>
-          <t>Upeneus vittatus</t>
+          <t>Upeneus vittatus</t>
         </is>
       </c>
       <c r="L630">
@@ -38223,7 +38223,7 @@
       </c>
       <c r="K631" t="inlineStr">
         <is>
-          <t>Upeneus vittatus</t>
+          <t>Upeneus vittatus</t>
         </is>
       </c>
       <c r="L631">
@@ -38283,7 +38283,7 @@
       </c>
       <c r="K632" t="inlineStr">
         <is>
-          <t>Upeneus vittatus</t>
+          <t>Upeneus vittatus</t>
         </is>
       </c>
       <c r="L632">
@@ -38343,7 +38343,7 @@
       </c>
       <c r="K633" t="inlineStr">
         <is>
-          <t>Upeneus vittatus</t>
+          <t>Upeneus vittatus</t>
         </is>
       </c>
       <c r="L633">
@@ -38403,7 +38403,7 @@
       </c>
       <c r="K634" t="inlineStr">
         <is>
-          <t>Upeneus vittatus</t>
+          <t>Upeneus vittatus</t>
         </is>
       </c>
       <c r="L634">
@@ -38463,7 +38463,7 @@
       </c>
       <c r="K635" t="inlineStr">
         <is>
-          <t>Upeneus vittatus</t>
+          <t>Upeneus vittatus</t>
         </is>
       </c>
       <c r="L635">
@@ -38523,7 +38523,7 @@
       </c>
       <c r="K636" t="inlineStr">
         <is>
-          <t>Upeneus vittatus</t>
+          <t>Upeneus vittatus</t>
         </is>
       </c>
       <c r="L636">
@@ -38583,7 +38583,7 @@
       </c>
       <c r="K637" t="inlineStr">
         <is>
-          <t>Upeneus vittatus</t>
+          <t>Upeneus vittatus</t>
         </is>
       </c>
       <c r="L637">
@@ -45663,7 +45663,7 @@
       </c>
       <c r="K755" t="inlineStr">
         <is>
-          <t>Cephalopholis spiloparaea</t>
+          <t>Cephalopholis spiloparaea</t>
         </is>
       </c>
       <c r="L755">
@@ -45903,7 +45903,7 @@
       </c>
       <c r="K759" t="inlineStr">
         <is>
-          <t>Epinephelus spilotoceps</t>
+          <t>Epinephelus spilotoceps</t>
         </is>
       </c>
       <c r="L759">
@@ -45963,7 +45963,7 @@
       </c>
       <c r="K760" t="inlineStr">
         <is>
-          <t>Epinephelus tauvina</t>
+          <t>Epinephelus tauvina</t>
         </is>
       </c>
       <c r="L760">
@@ -46023,7 +46023,7 @@
       </c>
       <c r="K761" t="inlineStr">
         <is>
-          <t>Epinephelus tauvina</t>
+          <t>Epinephelus tauvina</t>
         </is>
       </c>
       <c r="L761">
@@ -54723,7 +54723,7 @@
       </c>
       <c r="K906" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L906">
@@ -54783,7 +54783,7 @@
       </c>
       <c r="K907" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L907">
@@ -54843,7 +54843,7 @@
       </c>
       <c r="K908" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L908">
@@ -54903,7 +54903,7 @@
       </c>
       <c r="K909" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L909">
@@ -54963,7 +54963,7 @@
       </c>
       <c r="K910" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L910">
@@ -55023,7 +55023,7 @@
       </c>
       <c r="K911" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L911">
@@ -55083,7 +55083,7 @@
       </c>
       <c r="K912" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L912">
@@ -55143,7 +55143,7 @@
       </c>
       <c r="K913" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L913">
@@ -55203,7 +55203,7 @@
       </c>
       <c r="K914" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L914">
@@ -55263,7 +55263,7 @@
       </c>
       <c r="K915" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L915">
@@ -55323,7 +55323,7 @@
       </c>
       <c r="K916" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L916">
@@ -55383,7 +55383,7 @@
       </c>
       <c r="K917" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L917">
@@ -55443,7 +55443,7 @@
       </c>
       <c r="K918" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L918">
@@ -55503,7 +55503,7 @@
       </c>
       <c r="K919" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L919">
@@ -55563,7 +55563,7 @@
       </c>
       <c r="K920" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L920">
@@ -55623,7 +55623,7 @@
       </c>
       <c r="K921" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L921">
@@ -55683,7 +55683,7 @@
       </c>
       <c r="K922" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L922">
@@ -55743,7 +55743,7 @@
       </c>
       <c r="K923" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L923">
@@ -55803,7 +55803,7 @@
       </c>
       <c r="K924" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L924">
@@ -55863,7 +55863,7 @@
       </c>
       <c r="K925" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L925">
@@ -55923,7 +55923,7 @@
       </c>
       <c r="K926" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L926">
@@ -55983,7 +55983,7 @@
       </c>
       <c r="K927" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L927">
@@ -56043,7 +56043,7 @@
       </c>
       <c r="K928" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L928">
@@ -56103,7 +56103,7 @@
       </c>
       <c r="K929" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L929">
@@ -56163,7 +56163,7 @@
       </c>
       <c r="K930" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L930">
@@ -56223,7 +56223,7 @@
       </c>
       <c r="K931" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L931">
@@ -56283,7 +56283,7 @@
       </c>
       <c r="K932" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L932">
@@ -56343,7 +56343,7 @@
       </c>
       <c r="K933" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L933">
@@ -56403,7 +56403,7 @@
       </c>
       <c r="K934" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L934">
@@ -56463,7 +56463,7 @@
       </c>
       <c r="K935" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L935">
@@ -56523,7 +56523,7 @@
       </c>
       <c r="K936" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L936">
@@ -56583,7 +56583,7 @@
       </c>
       <c r="K937" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L937">
@@ -56643,7 +56643,7 @@
       </c>
       <c r="K938" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L938">
@@ -56703,7 +56703,7 @@
       </c>
       <c r="K939" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L939">
@@ -56763,7 +56763,7 @@
       </c>
       <c r="K940" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L940">
@@ -56823,7 +56823,7 @@
       </c>
       <c r="K941" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L941">
@@ -56883,7 +56883,7 @@
       </c>
       <c r="K942" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L942">
@@ -56943,7 +56943,7 @@
       </c>
       <c r="K943" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L943">
@@ -57003,7 +57003,7 @@
       </c>
       <c r="K944" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L944">
@@ -57063,7 +57063,7 @@
       </c>
       <c r="K945" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L945">
@@ -57123,7 +57123,7 @@
       </c>
       <c r="K946" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L946">
@@ -57183,7 +57183,7 @@
       </c>
       <c r="K947" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L947">
@@ -57243,7 +57243,7 @@
       </c>
       <c r="K948" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L948">
@@ -57303,7 +57303,7 @@
       </c>
       <c r="K949" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L949">
@@ -57363,7 +57363,7 @@
       </c>
       <c r="K950" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L950">
@@ -57423,7 +57423,7 @@
       </c>
       <c r="K951" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L951">
@@ -57483,7 +57483,7 @@
       </c>
       <c r="K952" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L952">
@@ -57543,7 +57543,7 @@
       </c>
       <c r="K953" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L953">
@@ -57603,7 +57603,7 @@
       </c>
       <c r="K954" t="inlineStr">
         <is>
-          <t>Sphyraena obtusata</t>
+          <t>Sphyraena obtusata</t>
         </is>
       </c>
       <c r="L954">
@@ -57663,7 +57663,7 @@
       </c>
       <c r="K955" t="inlineStr">
         <is>
-          <t>Saurida gracilis</t>
+          <t>Saurida gracilis</t>
         </is>
       </c>
       <c r="L955">

</xml_diff>

<commit_message>
updated analysis script and replaced species output files
</commit_message>
<xml_diff>
--- a/data/LengthData_20230712_EScleaned.xlsx
+++ b/data/LengthData_20230712_EScleaned.xlsx
@@ -44447,7 +44447,7 @@
       </c>
       <c r="G735" t="inlineStr">
         <is>
-          <t>Monofilament</t>
+          <t>Hand line</t>
         </is>
       </c>
       <c r="H735">
@@ -44507,7 +44507,7 @@
       </c>
       <c r="G736" t="inlineStr">
         <is>
-          <t>Monofilament</t>
+          <t>Hand line</t>
         </is>
       </c>
       <c r="H736">
@@ -44567,7 +44567,7 @@
       </c>
       <c r="G737" t="inlineStr">
         <is>
-          <t>Monofilament</t>
+          <t>Hand line</t>
         </is>
       </c>
       <c r="H737">
@@ -44627,7 +44627,7 @@
       </c>
       <c r="G738" t="inlineStr">
         <is>
-          <t>Monofilament</t>
+          <t>Hand line</t>
         </is>
       </c>
       <c r="H738">

</xml_diff>